<commit_message>
fix to tfidf preprocessing issue for context sentences; several small fixes and updates
</commit_message>
<xml_diff>
--- a/appendix/f1-macro-mean-difference.xlsx
+++ b/appendix/f1-macro-mean-difference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritzlaurer/Dropbox/PhD/Papers/nli/snellius/NLI-experiments/appendix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2123596B-8D9C-CC45-8502-1884F4036DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BC6FD0-64FC-B749-9C7A-D6C2E88499B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -620,6 +620,12 @@
         <v>3.9750000000000001E-2</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>12.3 - 7.2</f>
+        <v>5.1000000000000005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>